<commit_message>
report: Add CUDA eval section
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/test/cuda_threads.xlsx
+++ b/test/cuda_threads.xlsx
@@ -44,7 +44,7 @@
     <t>Occupancy</t>
   </si>
   <si>
-    <t>Max Warps</t>
+    <t>Blocked Warps</t>
   </si>
 </sst>
 </file>
@@ -80,8 +80,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,7 +364,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="40"/>
         <c:overlap val="100"/>
         <c:axId val="550123920"/>
         <c:axId val="550122280"/>
@@ -683,6 +684,45 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Occupancy &amp;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Blocked Warps </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>vs. Threads per Block</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -715,8 +755,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -733,17 +774,116 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-AEB6-4A0B-BB92-5371A861FD6E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-AEB6-4A0B-BB92-5371A861FD6E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-AEB6-4A0B-BB92-5371A861FD6E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$3:$A$9</c:f>
@@ -784,27 +924,26 @@
                   <c:v>3.13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>3.13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>6.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4372-4CEC-BBC4-1E9F8CAC85FE}"/>
@@ -819,17 +958,376 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:gapWidth val="27"/>
+        <c:overlap val="-25"/>
+        <c:axId val="531673336"/>
+        <c:axId val="531666448"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Blocked Warps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-AEB6-4A0B-BB92-5371A861FD6E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AEB6-4A0B-BB92-5371A861FD6E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="560160216"/>
-        <c:axId val="560162184"/>
+        <c:axId val="531655296"/>
+        <c:axId val="531649392"/>
       </c:lineChart>
+      <c:valAx>
+        <c:axId val="531666448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Occupancy (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="531673336"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:catAx>
-        <c:axId val="560160216"/>
+        <c:axId val="531673336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Threads per Block</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -867,36 +1365,84 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="560162184"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="531666448"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="560162184"/>
+        <c:axId val="531649392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Blocked Warps</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -926,10 +1472,26 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="560160216"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="531655296"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:catAx>
+        <c:axId val="531655296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="531649392"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -938,6 +1500,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2460,7 +3053,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2524,7 +3117,10 @@
         <v>963</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>3.13</v>
+      </c>
+      <c r="H4">
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2541,7 +3137,10 @@
         <v>724</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>6.25</v>
+      </c>
+      <c r="H5">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2558,7 +3157,10 @@
         <v>521</v>
       </c>
       <c r="G6">
-        <v>20</v>
+        <v>12.25</v>
+      </c>
+      <c r="H6">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2574,8 +3176,11 @@
       <c r="D7">
         <v>421.61</v>
       </c>
-      <c r="G7">
-        <v>40</v>
+      <c r="G7" s="1">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2591,8 +3196,11 @@
       <c r="D8">
         <v>425.82</v>
       </c>
-      <c r="G8">
-        <v>60</v>
+      <c r="G8" s="1">
+        <v>50</v>
+      </c>
+      <c r="H8" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2608,8 +3216,11 @@
       <c r="D9">
         <v>420</v>
       </c>
-      <c r="G9">
-        <v>80</v>
+      <c r="G9" s="1">
+        <v>50</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>